<commit_message>
update plan de pruebas
</commit_message>
<xml_diff>
--- a/Plan de Pruebas plantilla.xlsx
+++ b/Plan de Pruebas plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA6D5A-CD26-4BDE-A2BA-882D17067663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73361356-678A-4749-8F0D-0FA3C4AACDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>Click en Yes, click en Impressive y click en Yes</t>
   </si>
   <si>
-    <t>Comprobar que aparece como seleccionado Yes</t>
-  </si>
-  <si>
     <t>Elements_TC07</t>
   </si>
   <si>
@@ -299,10 +296,13 @@
     - Botón Click Me</t>
   </si>
   <si>
-    <t>Click en el botón Click Me, click derecho en el botón Right Click Me y doble click en el botón Double Click Me.</t>
+    <t>Comprobar que aparece un texto que indica que has hecho double click, right click y dynamic click.</t>
   </si>
   <si>
-    <t>Comprobar que aparece un texto que indica que has hecho double click, right click y dynamic click.</t>
+    <t>Comprobar que solo aparece como seleccionado el radio button Yes</t>
+  </si>
+  <si>
+    <t>Click izquierdo en el botón Click Me, click derecho en el botón Right Click Me y doble click izquierdo en el botón Double Click Me.</t>
   </si>
 </sst>
 </file>
@@ -597,49 +597,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -659,6 +616,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,7 +878,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -936,13 +936,13 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="167.25" customHeight="1" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="2">
         <v>1</v>
       </c>
@@ -976,9 +976,9 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="210" customHeight="1" thickBot="1">
-      <c r="A3" s="43"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="5">
         <v>2</v>
       </c>
@@ -1010,13 +1010,13 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="35" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2">
@@ -1052,9 +1052,9 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="180">
-      <c r="A5" s="42"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -1086,9 +1086,9 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="90">
-      <c r="A6" s="42"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -1120,9 +1120,9 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="10">
         <v>4</v>
       </c>
@@ -1155,14 +1155,14 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:26" ht="157.5" customHeight="1" thickBot="1">
+      <c r="A8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="35" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="3">
@@ -1197,10 +1197,10 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="180">
-      <c r="A9" s="32"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="34"/>
+    <row r="9" spans="1:26" ht="198" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="17">
         <v>2</v>
       </c>
@@ -1231,10 +1231,10 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="30">
-      <c r="A10" s="32"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="34"/>
+    <row r="10" spans="1:26" ht="36" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="17">
         <v>3</v>
       </c>
@@ -1265,10 +1265,10 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="35"/>
+    <row r="11" spans="1:26" ht="69" customHeight="1" thickBot="1">
+      <c r="A11" s="42"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="19">
         <v>4</v>
       </c>
@@ -1300,13 +1300,13 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="159.75" customHeight="1">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="15">
@@ -1315,7 +1315,7 @@
       <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="28" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -1342,9 +1342,9 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="200.25" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="17">
         <v>2</v>
       </c>
@@ -1376,9 +1376,9 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="33" customHeight="1">
-      <c r="A14" s="32"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="17">
         <v>3</v>
       </c>
@@ -1410,9 +1410,9 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="83.25" customHeight="1" thickBot="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="19">
         <v>4</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="F15" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="46"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1444,13 +1444,13 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="155.25" customHeight="1" thickBot="1">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="15">
@@ -1486,9 +1486,9 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" ht="204" customHeight="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="17">
         <v>2</v>
       </c>
@@ -1520,9 +1520,9 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="30">
-      <c r="A18" s="32"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="17">
         <v>3</v>
       </c>
@@ -1554,19 +1554,19 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34">
+      <c r="A19" s="41"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36">
         <v>4</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="29"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1588,13 +1588,13 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="29"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="48"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1616,13 +1616,13 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="29"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -1644,13 +1644,13 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A22" s="32"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="29"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -1672,13 +1672,13 @@
       <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="30"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1700,13 +1700,13 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="156" customHeight="1" thickBot="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="15">
@@ -1742,9 +1742,9 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:26" ht="201" customHeight="1">
-      <c r="A25" s="32"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="17">
         <v>2</v>
       </c>
@@ -1776,9 +1776,9 @@
       <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:26" ht="60">
-      <c r="A26" s="32"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="17">
         <v>3</v>
       </c>
@@ -1810,19 +1810,19 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="32"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34">
+      <c r="A27" s="41"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36">
         <v>4</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="27" t="s">
-        <v>39</v>
+      <c r="F27" s="46" t="s">
+        <v>58</v>
       </c>
-      <c r="G27" s="29"/>
+      <c r="G27" s="48"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -1844,13 +1844,13 @@
       <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="32"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="29"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="48"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -1872,13 +1872,13 @@
       <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="32"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="29"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="48"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -1900,13 +1900,13 @@
       <c r="Z29" s="5"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="32"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="29"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="48"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -1928,13 +1928,13 @@
       <c r="Z30" s="5"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="30"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -1956,13 +1956,13 @@
       <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:26" ht="159.75" customHeight="1" thickBot="1">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="15">
@@ -1998,9 +1998,9 @@
       <c r="Z32" s="5"/>
     </row>
     <row r="33" spans="1:26" ht="200.25" customHeight="1">
-      <c r="A33" s="32"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="17">
         <v>2</v>
       </c>
@@ -2032,17 +2032,17 @@
       <c r="Z33" s="5"/>
     </row>
     <row r="34" spans="1:26" ht="90">
-      <c r="A34" s="32"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="17">
         <v>3</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="5"/>
@@ -2066,19 +2066,19 @@
       <c r="Z34" s="5"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="32"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34">
+      <c r="A35" s="41"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36">
         <v>4</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" s="29"/>
+      <c r="G35" s="48"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -2100,13 +2100,13 @@
       <c r="Z35" s="5"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="32"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="29"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="48"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -2128,13 +2128,13 @@
       <c r="Z36" s="5"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="32"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="29"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="48"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -2156,13 +2156,13 @@
       <c r="Z37" s="5"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="32"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="29"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="48"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
@@ -2184,13 +2184,13 @@
       <c r="Z38" s="5"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A39" s="33"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="30"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="49"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -2212,13 +2212,13 @@
       <c r="Z39" s="5"/>
     </row>
     <row r="40" spans="1:26" ht="157.5" customHeight="1" thickBot="1">
-      <c r="A40" s="37" t="s">
-        <v>48</v>
+      <c r="A40" s="50" t="s">
+        <v>47</v>
       </c>
-      <c r="B40" s="36" t="s">
-        <v>41</v>
+      <c r="B40" s="51" t="s">
+        <v>40</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="15">
@@ -2254,9 +2254,9 @@
       <c r="Z40" s="5"/>
     </row>
     <row r="41" spans="1:26" ht="200.25" customHeight="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="17">
         <v>2</v>
       </c>
@@ -2288,17 +2288,17 @@
       <c r="Z41" s="5"/>
     </row>
     <row r="42" spans="1:26" ht="96.75" customHeight="1">
-      <c r="A42" s="32"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="17">
         <v>3</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="5"/>
@@ -2322,20 +2322,20 @@
       <c r="Z42" s="5"/>
     </row>
     <row r="43" spans="1:26" ht="225" customHeight="1" thickBot="1">
-      <c r="A43" s="32"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="19">
         <v>4</v>
       </c>
-      <c r="E43" s="48" t="s">
-        <v>46</v>
+      <c r="E43" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -2358,25 +2358,25 @@
       <c r="Z43" s="5"/>
     </row>
     <row r="44" spans="1:26" ht="164.25" customHeight="1">
-      <c r="A44" s="37" t="s">
-        <v>49</v>
+      <c r="A44" s="50" t="s">
+        <v>48</v>
       </c>
-      <c r="B44" s="36" t="s">
-        <v>41</v>
+      <c r="B44" s="51" t="s">
+        <v>40</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="22">
         <v>1</v>
       </c>
-      <c r="E44" s="45" t="s">
+      <c r="E44" s="28" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="49" t="s">
+      <c r="G44" s="32" t="s">
         <v>11</v>
       </c>
       <c r="H44" s="5"/>
@@ -2400,9 +2400,9 @@
       <c r="Z44" s="5"/>
     </row>
     <row r="45" spans="1:26" ht="201.75" customHeight="1">
-      <c r="A45" s="32"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="17">
         <v>2</v>
       </c>
@@ -2412,7 +2412,7 @@
       <c r="F45" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G45" s="47"/>
+      <c r="G45" s="30"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
@@ -2434,19 +2434,19 @@
       <c r="Z45" s="5"/>
     </row>
     <row r="46" spans="1:26" ht="90">
-      <c r="A46" s="32"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="17">
         <v>3</v>
       </c>
       <c r="E46" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F46" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G46" s="47"/>
+      <c r="G46" s="30"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -2468,20 +2468,20 @@
       <c r="Z46" s="5"/>
     </row>
     <row r="47" spans="1:26" ht="210.75" thickBot="1">
-      <c r="A47" s="33"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="19">
         <v>4</v>
       </c>
-      <c r="E47" s="48" t="s">
-        <v>50</v>
+      <c r="E47" s="31" t="s">
+        <v>49</v>
       </c>
       <c r="F47" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="33" t="s">
         <v>52</v>
-      </c>
-      <c r="G47" s="50" t="s">
-        <v>53</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2504,25 +2504,25 @@
       <c r="Z47" s="5"/>
     </row>
     <row r="48" spans="1:26" ht="159.75" customHeight="1">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="22">
         <v>1</v>
       </c>
-      <c r="E48" s="45" t="s">
+      <c r="E48" s="28" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G48" s="49" t="s">
+      <c r="G48" s="32" t="s">
         <v>11</v>
       </c>
       <c r="H48" s="5"/>
@@ -2546,9 +2546,9 @@
       <c r="Z48" s="5"/>
     </row>
     <row r="49" spans="1:26" ht="180">
-      <c r="A49" s="32"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
       <c r="D49" s="17">
         <v>2</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="F49" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G49" s="47"/>
+      <c r="G49" s="30"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -2580,19 +2580,19 @@
       <c r="Z49" s="5"/>
     </row>
     <row r="50" spans="1:26" ht="60">
-      <c r="A50" s="32"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
       <c r="D50" s="17">
         <v>3</v>
       </c>
       <c r="E50" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F50" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="G50" s="47"/>
+      <c r="G50" s="30"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -2613,20 +2613,20 @@
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
     </row>
-    <row r="51" spans="1:26" ht="45">
-      <c r="A51" s="33"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
+    <row r="51" spans="1:26" ht="60">
+      <c r="A51" s="42"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="19">
         <v>4</v>
       </c>
-      <c r="E51" s="51" t="s">
-        <v>58</v>
+      <c r="E51" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
-      <c r="G51" s="50"/>
+      <c r="G51" s="33"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -2722,7 +2722,7 @@
     <row r="55" spans="1:26">
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
-      <c r="G55" s="47"/>
+      <c r="G55" s="30"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -2750,7 +2750,7 @@
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
       <c r="F56" s="16"/>
-      <c r="G56" s="44"/>
+      <c r="G56" s="27"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
@@ -29172,7 +29172,6 @@
     <mergeCell ref="C24:C31"/>
     <mergeCell ref="D27:D31"/>
     <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F19:F23"/>
     <mergeCell ref="G19:G23"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B12:B15"/>
@@ -29182,15 +29181,16 @@
     <mergeCell ref="C16:C23"/>
     <mergeCell ref="D19:D23"/>
     <mergeCell ref="E19:E23"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C7"/>
+    <mergeCell ref="F19:F23"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>